<commit_message>
added in rest of data and added in WJ correlation testing
</commit_message>
<xml_diff>
--- a/bko2 age table.xlsx
+++ b/bko2 age table.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisabeth/Desktop/UMASS/BKonline data/BK-Online-Replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF172D3D-1EE6-364C-91FE-5DD5EEA26C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A3CC53-3CFA-934F-9327-04BCAFA19E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="1500" windowWidth="28700" windowHeight="15440" xr2:uid="{C0172237-591B-2148-8687-3BFAE2F61C1B}"/>
+    <workbookView xWindow="29740" yWindow="500" windowWidth="28700" windowHeight="15440" xr2:uid="{C0172237-591B-2148-8687-3BFAE2F61C1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -216,13 +216,43 @@
   </si>
   <si>
     <t>bkp118</t>
+  </si>
+  <si>
+    <t>bkp119</t>
+  </si>
+  <si>
+    <t>bkp120</t>
+  </si>
+  <si>
+    <t>bkp059</t>
+  </si>
+  <si>
+    <t>bkp060</t>
+  </si>
+  <si>
+    <t>bkp061</t>
+  </si>
+  <si>
+    <t>bkp062</t>
+  </si>
+  <si>
+    <t>bkp063</t>
+  </si>
+  <si>
+    <t>bkp064</t>
+  </si>
+  <si>
+    <t>bkp065</t>
+  </si>
+  <si>
+    <t>bkp066</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -238,6 +268,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,10 +300,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -583,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D931D60F-2CDE-A44B-83AE-00FB255FCEBC}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1000,98 +1040,98 @@
     </row>
     <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="B38" s="3">
+        <v>6</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="B39" s="3">
+        <v>7</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="B40" s="3">
+        <v>6</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="B41" s="3">
+        <v>8</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="B42" s="3">
+        <v>8</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="B43" s="3">
+        <v>8</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="B44" s="3">
+        <v>7</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
+        <v>69</v>
+      </c>
+      <c r="B45" s="3">
+        <v>7</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>56</v>
@@ -1099,10 +1139,10 @@
     </row>
     <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>56</v>
@@ -1110,10 +1150,10 @@
     </row>
     <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>56</v>
@@ -1121,10 +1161,10 @@
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>56</v>
@@ -1132,10 +1172,10 @@
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>56</v>
@@ -1143,10 +1183,10 @@
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>56</v>
@@ -1154,10 +1194,10 @@
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>56</v>
@@ -1165,10 +1205,10 @@
     </row>
     <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>56</v>
@@ -1176,10 +1216,10 @@
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>56</v>
@@ -1187,18 +1227,128 @@
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55">
+        <v>18</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56">
+        <v>18</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57">
+        <v>18</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58">
+        <v>18</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59">
+        <v>18</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B60">
+        <v>18</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61">
+        <v>18</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B62">
+        <v>18</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="B63">
+        <v>18</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64">
+        <v>18</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65">
+        <v>18</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C54">
-    <sortCondition ref="A2:A54"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C65">
+    <sortCondition ref="A2:A65"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>